<commit_message>
Fix: Improve find_best_mapping to choose longest matching mapping
- Modified find_best_mapping() to select the mapping with the longest name
  when multiple mappings match (exact match or longest prefix)
- Only return None if multiple mappings have the same maximum length (real conflict)
- This fixes transactions that were incorrectly left unclassified when a better
  mapping existed (e.g., exact match vs prefix match)
- Updated documentation in IMPLEMENTATION_PLAN_PHASE_5.md
</commit_message>
<xml_diff>
--- a/backend/data/input/trades/mappings_vf.xlsx
+++ b/backend/data/input/trades/mappings_vf.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/louisgarnier/Desktop/LMNP/Evry/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D95D478-D03A-CE4E-9206-944CFE706C5C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F68D52A6-6D40-344C-9407-E11DBF860ACA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-19280" yWindow="-26620" windowWidth="52740" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="11120" yWindow="-26620" windowWidth="52740" windowHeight="26620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Mappings" sheetId="1" r:id="rId1"/>
@@ -515,12 +515,6 @@
     <t>Frais de gestion locative</t>
   </si>
   <si>
-    <t>Emprunt immobilier</t>
-  </si>
-  <si>
-    <t>Emprunt et assurance emprunteur</t>
-  </si>
-  <si>
     <t>Équipement</t>
   </si>
   <si>
@@ -579,19 +573,31 @@
   </si>
   <si>
     <t>Dettes financières (emprunt bancaire)</t>
+  </si>
+  <si>
+    <t>Paiement mensualites credit (capital, interet, assurance)</t>
+  </si>
+  <si>
+    <t>Mensualités</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Helvetica"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -614,8 +620,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -958,7 +965,7 @@
   <dimension ref="A1:D135"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -966,7 +973,6 @@
     <col min="1" max="1" width="30.83203125" customWidth="1"/>
     <col min="2" max="2" width="38.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="26.1640625" customWidth="1"/>
-    <col min="7" max="7" width="11" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -988,13 +994,13 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C2" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D2" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -1008,7 +1014,7 @@
         <v>150</v>
       </c>
       <c r="D3" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -1016,41 +1022,41 @@
         <v>6</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C4" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D4" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>160</v>
+      <c r="B5" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C5" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="D5" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>160</v>
+      <c r="B6" s="1" t="s">
+        <v>179</v>
       </c>
       <c r="C6" t="s">
-        <v>159</v>
+        <v>180</v>
       </c>
       <c r="D6" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -1058,13 +1064,13 @@
         <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C7" t="s">
         <v>153</v>
       </c>
       <c r="D7" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -1072,13 +1078,13 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C8" t="s">
         <v>153</v>
       </c>
       <c r="D8" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -1086,13 +1092,13 @@
         <v>11</v>
       </c>
       <c r="B9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C9" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D9" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.2">
@@ -1100,13 +1106,13 @@
         <v>12</v>
       </c>
       <c r="B10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C10" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D10" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.2">
@@ -1120,7 +1126,7 @@
         <v>155</v>
       </c>
       <c r="D11" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.2">
@@ -1134,7 +1140,7 @@
         <v>141</v>
       </c>
       <c r="D12" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.2">
@@ -1148,7 +1154,7 @@
         <v>153</v>
       </c>
       <c r="D13" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.2">
@@ -1156,13 +1162,13 @@
         <v>17</v>
       </c>
       <c r="B14" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D14" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.2">
@@ -1170,13 +1176,13 @@
         <v>18</v>
       </c>
       <c r="B15" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C15" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D15" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.2">
@@ -1190,7 +1196,7 @@
         <v>153</v>
       </c>
       <c r="D16" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.2">
@@ -1198,27 +1204,27 @@
         <v>20</v>
       </c>
       <c r="B17" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D17" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>21</v>
       </c>
-      <c r="B18" t="s">
+      <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="19" spans="1:4" x14ac:dyDescent="0.2">
@@ -1226,13 +1232,13 @@
         <v>23</v>
       </c>
       <c r="B19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C19" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D19" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="20" spans="1:4" x14ac:dyDescent="0.2">
@@ -1240,13 +1246,13 @@
         <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C20" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D20" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="21" spans="1:4" x14ac:dyDescent="0.2">
@@ -1254,13 +1260,13 @@
         <v>25</v>
       </c>
       <c r="B21" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D21" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="22" spans="1:4" x14ac:dyDescent="0.2">
@@ -1268,13 +1274,13 @@
         <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D22" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="23" spans="1:4" x14ac:dyDescent="0.2">
@@ -1282,13 +1288,13 @@
         <v>27</v>
       </c>
       <c r="B23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C23" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D23" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.2">
@@ -1296,13 +1302,13 @@
         <v>28</v>
       </c>
       <c r="B24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C24" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D24" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.2">
@@ -1310,13 +1316,13 @@
         <v>29</v>
       </c>
       <c r="B25" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D25" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.2">
@@ -1327,10 +1333,10 @@
         <v>143</v>
       </c>
       <c r="C26" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D26" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="27" spans="1:4" x14ac:dyDescent="0.2">
@@ -1341,10 +1347,10 @@
         <v>143</v>
       </c>
       <c r="C27" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D27" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.2">
@@ -1352,13 +1358,13 @@
         <v>32</v>
       </c>
       <c r="B28" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C28" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D28" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="29" spans="1:4" x14ac:dyDescent="0.2">
@@ -1372,7 +1378,7 @@
         <v>150</v>
       </c>
       <c r="D29" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.2">
@@ -1383,10 +1389,10 @@
         <v>144</v>
       </c>
       <c r="C30" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D30" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.2">
@@ -1394,13 +1400,13 @@
         <v>35</v>
       </c>
       <c r="B31" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D31" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.2">
@@ -1408,13 +1414,13 @@
         <v>36</v>
       </c>
       <c r="B32" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D32" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="33" spans="1:4" x14ac:dyDescent="0.2">
@@ -1422,13 +1428,13 @@
         <v>37</v>
       </c>
       <c r="B33" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C33" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D33" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="34" spans="1:4" x14ac:dyDescent="0.2">
@@ -1442,7 +1448,7 @@
         <v>141</v>
       </c>
       <c r="D34" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="35" spans="1:4" x14ac:dyDescent="0.2">
@@ -1450,13 +1456,13 @@
         <v>39</v>
       </c>
       <c r="B35" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D35" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="36" spans="1:4" x14ac:dyDescent="0.2">
@@ -1464,13 +1470,13 @@
         <v>40</v>
       </c>
       <c r="B36" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D36" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="37" spans="1:4" x14ac:dyDescent="0.2">
@@ -1478,13 +1484,13 @@
         <v>41</v>
       </c>
       <c r="B37" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D37" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="1:4" x14ac:dyDescent="0.2">
@@ -1498,7 +1504,7 @@
         <v>153</v>
       </c>
       <c r="D38" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="39" spans="1:4" x14ac:dyDescent="0.2">
@@ -1506,13 +1512,13 @@
         <v>43</v>
       </c>
       <c r="B39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C39" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D39" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="40" spans="1:4" x14ac:dyDescent="0.2">
@@ -1520,13 +1526,13 @@
         <v>44</v>
       </c>
       <c r="B40" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D40" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="41" spans="1:4" x14ac:dyDescent="0.2">
@@ -1540,7 +1546,7 @@
         <v>156</v>
       </c>
       <c r="D41" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="42" spans="1:4" x14ac:dyDescent="0.2">
@@ -1554,7 +1560,7 @@
         <v>141</v>
       </c>
       <c r="D42" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="43" spans="1:4" x14ac:dyDescent="0.2">
@@ -1562,13 +1568,13 @@
         <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C43" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D43" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="44" spans="1:4" x14ac:dyDescent="0.2">
@@ -1576,13 +1582,13 @@
         <v>48</v>
       </c>
       <c r="B44" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C44" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D44" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.2">
@@ -1590,13 +1596,13 @@
         <v>49</v>
       </c>
       <c r="B45" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C45" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D45" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.2">
@@ -1604,13 +1610,13 @@
         <v>50</v>
       </c>
       <c r="B46" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C46" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D46" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.2">
@@ -1618,13 +1624,13 @@
         <v>51</v>
       </c>
       <c r="B47" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="C47" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="D47" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.2">
@@ -1638,7 +1644,7 @@
         <v>156</v>
       </c>
       <c r="D48" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.2">
@@ -1652,7 +1658,7 @@
         <v>153</v>
       </c>
       <c r="D49" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.2">
@@ -1660,13 +1666,13 @@
         <v>54</v>
       </c>
       <c r="B50" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C50" t="s">
         <v>153</v>
       </c>
       <c r="D50" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.2">
@@ -1674,13 +1680,13 @@
         <v>55</v>
       </c>
       <c r="B51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C51" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D51" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.2">
@@ -1694,7 +1700,7 @@
         <v>141</v>
       </c>
       <c r="D52" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.2">
@@ -1702,13 +1708,13 @@
         <v>57</v>
       </c>
       <c r="B53" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C53" t="s">
         <v>153</v>
       </c>
       <c r="D53" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.2">
@@ -1719,10 +1725,10 @@
         <v>144</v>
       </c>
       <c r="C54" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D54" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.2">
@@ -1730,13 +1736,13 @@
         <v>59</v>
       </c>
       <c r="B55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C55" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D55" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.2">
@@ -1744,13 +1750,13 @@
         <v>60</v>
       </c>
       <c r="B56" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C56" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D56" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.2">
@@ -1764,7 +1770,7 @@
         <v>141</v>
       </c>
       <c r="D57" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.2">
@@ -1775,10 +1781,10 @@
         <v>142</v>
       </c>
       <c r="C58" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D58" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.2">
@@ -1789,10 +1795,10 @@
         <v>140</v>
       </c>
       <c r="C59" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D59" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.2">
@@ -1800,13 +1806,13 @@
         <v>64</v>
       </c>
       <c r="B60" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C60" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="D60" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="61" spans="1:4" x14ac:dyDescent="0.2">
@@ -1814,13 +1820,13 @@
         <v>65</v>
       </c>
       <c r="B61" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C61" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D61" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="62" spans="1:4" x14ac:dyDescent="0.2">
@@ -1834,7 +1840,7 @@
         <v>150</v>
       </c>
       <c r="D62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="63" spans="1:4" x14ac:dyDescent="0.2">
@@ -1842,13 +1848,13 @@
         <v>67</v>
       </c>
       <c r="B63" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C63" t="s">
         <v>153</v>
       </c>
       <c r="D63" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="64" spans="1:4" x14ac:dyDescent="0.2">
@@ -1862,7 +1868,7 @@
         <v>155</v>
       </c>
       <c r="D64" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="65" spans="1:4" x14ac:dyDescent="0.2">
@@ -1876,7 +1882,7 @@
         <v>141</v>
       </c>
       <c r="D65" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="66" spans="1:4" x14ac:dyDescent="0.2">
@@ -1890,7 +1896,7 @@
         <v>150</v>
       </c>
       <c r="D66" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="67" spans="1:4" x14ac:dyDescent="0.2">
@@ -1898,27 +1904,27 @@
         <v>70</v>
       </c>
       <c r="B67" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C67" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D67" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="68" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>71</v>
       </c>
-      <c r="B68" t="s">
-        <v>177</v>
+      <c r="B68" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C68" t="s">
         <v>72</v>
       </c>
       <c r="D68" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="69" spans="1:4" x14ac:dyDescent="0.2">
@@ -1926,41 +1932,41 @@
         <v>73</v>
       </c>
       <c r="B69" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C69" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D69" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>74</v>
       </c>
-      <c r="B70" t="s">
+      <c r="B70" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C70" t="s">
         <v>72</v>
       </c>
       <c r="D70" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="71" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>75</v>
       </c>
-      <c r="B71" t="s">
-        <v>177</v>
+      <c r="B71" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C71" t="s">
         <v>72</v>
       </c>
       <c r="D71" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.2">
@@ -1968,13 +1974,13 @@
         <v>76</v>
       </c>
       <c r="B72" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C72" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D72" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.2">
@@ -1988,7 +1994,7 @@
         <v>156</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="74" spans="1:4" x14ac:dyDescent="0.2">
@@ -1996,13 +2002,13 @@
         <v>79</v>
       </c>
       <c r="B74" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C74" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D74" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="75" spans="1:4" x14ac:dyDescent="0.2">
@@ -2016,7 +2022,7 @@
         <v>146</v>
       </c>
       <c r="D75" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="76" spans="1:4" x14ac:dyDescent="0.2">
@@ -2030,7 +2036,7 @@
         <v>156</v>
       </c>
       <c r="D76" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="77" spans="1:4" x14ac:dyDescent="0.2">
@@ -2038,13 +2044,13 @@
         <v>81</v>
       </c>
       <c r="B77" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C77" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D77" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="78" spans="1:4" x14ac:dyDescent="0.2">
@@ -2052,13 +2058,13 @@
         <v>82</v>
       </c>
       <c r="B78" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C78" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D78" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="79" spans="1:4" x14ac:dyDescent="0.2">
@@ -2066,13 +2072,13 @@
         <v>83</v>
       </c>
       <c r="B79" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C79" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D79" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="80" spans="1:4" x14ac:dyDescent="0.2">
@@ -2086,7 +2092,7 @@
         <v>156</v>
       </c>
       <c r="D80" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="81" spans="1:4" x14ac:dyDescent="0.2">
@@ -2100,7 +2106,7 @@
         <v>156</v>
       </c>
       <c r="D81" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="82" spans="1:4" x14ac:dyDescent="0.2">
@@ -2108,13 +2114,13 @@
         <v>86</v>
       </c>
       <c r="B82" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C82" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D82" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="83" spans="1:4" x14ac:dyDescent="0.2">
@@ -2122,13 +2128,13 @@
         <v>87</v>
       </c>
       <c r="B83" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C83" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D83" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="84" spans="1:4" x14ac:dyDescent="0.2">
@@ -2136,13 +2142,13 @@
         <v>88</v>
       </c>
       <c r="B84" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C84" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D84" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="85" spans="1:4" x14ac:dyDescent="0.2">
@@ -2150,13 +2156,13 @@
         <v>89</v>
       </c>
       <c r="B85" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D85" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="86" spans="1:4" x14ac:dyDescent="0.2">
@@ -2164,13 +2170,13 @@
         <v>90</v>
       </c>
       <c r="B86" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C86" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D86" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="87" spans="1:4" x14ac:dyDescent="0.2">
@@ -2178,13 +2184,13 @@
         <v>91</v>
       </c>
       <c r="B87" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C87" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D87" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.2">
@@ -2192,13 +2198,13 @@
         <v>92</v>
       </c>
       <c r="B88" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C88" t="s">
         <v>153</v>
       </c>
       <c r="D88" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="89" spans="1:4" x14ac:dyDescent="0.2">
@@ -2212,21 +2218,21 @@
         <v>156</v>
       </c>
       <c r="D89" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A90" t="s">
         <v>94</v>
       </c>
-      <c r="B90" t="s">
+      <c r="B90" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C90" t="s">
         <v>72</v>
       </c>
       <c r="D90" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="91" spans="1:4" x14ac:dyDescent="0.2">
@@ -2234,69 +2240,69 @@
         <v>95</v>
       </c>
       <c r="B91" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="C91" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="D91" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="92" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A92" t="s">
         <v>96</v>
       </c>
-      <c r="B92" t="s">
-        <v>177</v>
+      <c r="B92" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C92" t="s">
         <v>72</v>
       </c>
       <c r="D92" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="93" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A93" t="s">
         <v>97</v>
       </c>
-      <c r="B93" t="s">
-        <v>177</v>
+      <c r="B93" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C93" t="s">
         <v>72</v>
       </c>
       <c r="D93" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A94" t="s">
         <v>98</v>
       </c>
-      <c r="B94" t="s">
-        <v>177</v>
+      <c r="B94" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C94" t="s">
         <v>72</v>
       </c>
       <c r="D94" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A95" t="s">
         <v>99</v>
       </c>
-      <c r="B95" t="s">
-        <v>177</v>
+      <c r="B95" s="1" t="s">
+        <v>175</v>
       </c>
       <c r="C95" t="s">
         <v>72</v>
       </c>
       <c r="D95" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.2">
@@ -2304,13 +2310,13 @@
         <v>100</v>
       </c>
       <c r="B96" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C96" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D96" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="97" spans="1:4" x14ac:dyDescent="0.2">
@@ -2318,13 +2324,13 @@
         <v>101</v>
       </c>
       <c r="B97" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C97" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D97" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="98" spans="1:4" x14ac:dyDescent="0.2">
@@ -2338,7 +2344,7 @@
         <v>156</v>
       </c>
       <c r="D98" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="99" spans="1:4" x14ac:dyDescent="0.2">
@@ -2352,7 +2358,7 @@
         <v>156</v>
       </c>
       <c r="D99" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="100" spans="1:4" x14ac:dyDescent="0.2">
@@ -2366,7 +2372,7 @@
         <v>156</v>
       </c>
       <c r="D100" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="101" spans="1:4" x14ac:dyDescent="0.2">
@@ -2380,7 +2386,7 @@
         <v>156</v>
       </c>
       <c r="D101" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="102" spans="1:4" x14ac:dyDescent="0.2">
@@ -2388,13 +2394,13 @@
         <v>106</v>
       </c>
       <c r="B102" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C102" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D102" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="103" spans="1:4" x14ac:dyDescent="0.2">
@@ -2402,13 +2408,13 @@
         <v>107</v>
       </c>
       <c r="B103" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C103" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D103" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="104" spans="1:4" x14ac:dyDescent="0.2">
@@ -2416,13 +2422,13 @@
         <v>108</v>
       </c>
       <c r="B104" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C104" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D104" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="105" spans="1:4" x14ac:dyDescent="0.2">
@@ -2430,13 +2436,13 @@
         <v>109</v>
       </c>
       <c r="B105" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C105" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D105" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="106" spans="1:4" x14ac:dyDescent="0.2">
@@ -2444,13 +2450,13 @@
         <v>110</v>
       </c>
       <c r="B106" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D106" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="107" spans="1:4" x14ac:dyDescent="0.2">
@@ -2464,7 +2470,7 @@
         <v>156</v>
       </c>
       <c r="D107" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="108" spans="1:4" x14ac:dyDescent="0.2">
@@ -2478,7 +2484,7 @@
         <v>156</v>
       </c>
       <c r="D108" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="109" spans="1:4" x14ac:dyDescent="0.2">
@@ -2492,7 +2498,7 @@
         <v>156</v>
       </c>
       <c r="D109" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="110" spans="1:4" x14ac:dyDescent="0.2">
@@ -2506,7 +2512,7 @@
         <v>156</v>
       </c>
       <c r="D110" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="111" spans="1:4" x14ac:dyDescent="0.2">
@@ -2514,13 +2520,13 @@
         <v>115</v>
       </c>
       <c r="B111" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="C111" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D111" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="112" spans="1:4" x14ac:dyDescent="0.2">
@@ -2534,7 +2540,7 @@
         <v>156</v>
       </c>
       <c r="D112" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="113" spans="1:4" x14ac:dyDescent="0.2">
@@ -2545,10 +2551,10 @@
         <v>142</v>
       </c>
       <c r="C113" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D113" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="114" spans="1:4" x14ac:dyDescent="0.2">
@@ -2559,10 +2565,10 @@
         <v>140</v>
       </c>
       <c r="C114" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D114" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.2">
@@ -2573,10 +2579,10 @@
         <v>144</v>
       </c>
       <c r="C115" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
       <c r="D115" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="116" spans="1:4" x14ac:dyDescent="0.2">
@@ -2590,7 +2596,7 @@
         <v>141</v>
       </c>
       <c r="D116" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.2">
@@ -2598,13 +2604,13 @@
         <v>121</v>
       </c>
       <c r="B117" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C117" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="D117" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="118" spans="1:4" x14ac:dyDescent="0.2">
@@ -2612,13 +2618,13 @@
         <v>122</v>
       </c>
       <c r="B118" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C118" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D118" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="119" spans="1:4" x14ac:dyDescent="0.2">
@@ -2632,7 +2638,7 @@
         <v>153</v>
       </c>
       <c r="D119" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="120" spans="1:4" x14ac:dyDescent="0.2">
@@ -2646,7 +2652,7 @@
         <v>141</v>
       </c>
       <c r="D120" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.2">
@@ -2660,7 +2666,7 @@
         <v>141</v>
       </c>
       <c r="D121" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.2">
@@ -2668,13 +2674,13 @@
         <v>126</v>
       </c>
       <c r="B122" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C122" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D122" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.2">
@@ -2682,13 +2688,13 @@
         <v>127</v>
       </c>
       <c r="B123" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C123" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D123" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.2">
@@ -2702,7 +2708,7 @@
         <v>153</v>
       </c>
       <c r="D124" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.2">
@@ -2716,7 +2722,7 @@
         <v>153</v>
       </c>
       <c r="D125" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.2">
@@ -2724,13 +2730,13 @@
         <v>130</v>
       </c>
       <c r="B126" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C126" t="s">
         <v>153</v>
       </c>
       <c r="D126" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.2">
@@ -2744,7 +2750,7 @@
         <v>141</v>
       </c>
       <c r="D127" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.2">
@@ -2758,7 +2764,7 @@
         <v>141</v>
       </c>
       <c r="D128" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.2">
@@ -2772,7 +2778,7 @@
         <v>153</v>
       </c>
       <c r="D129" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.2">
@@ -2780,69 +2786,69 @@
         <v>134</v>
       </c>
       <c r="B130" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C130" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D130" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A131" t="s">
         <v>135</v>
       </c>
-      <c r="B131" t="s">
+      <c r="B131" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C131" t="s">
         <v>72</v>
       </c>
       <c r="D131" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="132" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A132" t="s">
         <v>136</v>
       </c>
-      <c r="B132" t="s">
+      <c r="B132" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C132" t="s">
         <v>72</v>
       </c>
       <c r="D132" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A133" t="s">
         <v>137</v>
       </c>
-      <c r="B133" t="s">
+      <c r="B133" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C133" t="s">
         <v>72</v>
       </c>
       <c r="D133" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="134" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A134" t="s">
         <v>138</v>
       </c>
-      <c r="B134" t="s">
+      <c r="B134" s="1" t="s">
         <v>145</v>
       </c>
       <c r="C134" t="s">
         <v>72</v>
       </c>
       <c r="D134" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="135" spans="1:4" x14ac:dyDescent="0.2">
@@ -2850,13 +2856,13 @@
         <v>139</v>
       </c>
       <c r="B135" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C135" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="D135" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
     </row>
   </sheetData>

</xml_diff>